<commit_message>
example cell number as interface
</commit_message>
<xml_diff>
--- a/example/config/ai_行为/ai行为.xlsx
+++ b/example/config/ai_行为/ai行为.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20374"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mygithub\configgen\example\config\ai_行为\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\work\mygit\cfggen\example\config\ai_行为\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6CB45F7-F81F-4A41-B863-40FCF8543EB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D17AE943-A970-46DB-AD7D-607DEF58D9D9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5430" yWindow="3810" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,6 +19,7 @@
     <sheet name="AI_ACTION_中文测试" sheetId="4" r:id="rId4"/>
     <sheet name="AI_ACTION_1_继续测试" sheetId="6" r:id="rId5"/>
     <sheet name="说明" sheetId="3" r:id="rId6"/>
+    <sheet name="TriggerTickType" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">AI_ACTION_中文测试!$C:$C</definedName>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="189">
   <si>
     <t>sheet</t>
   </si>
@@ -654,6 +655,70 @@
 再来一行</t>
     <phoneticPr fontId="13" type="noConversion"/>
   </si>
+  <si>
+    <t>enumName</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>枚举名称</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>策划注释</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>参数列表</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>ConstValue</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>value:int</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>ByLevel</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>init:int</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>ByServerUpDay</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>角色等级相关</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>服务器启动天数</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>coefficient1:float</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>coefficient2:falot</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>coefficient:float</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>ByLevel(100, 0.1)</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>ByServerUpDay(10, 0.1, 0.2)</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -662,7 +727,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="##0"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -765,6 +830,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
@@ -916,7 +989,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1064,6 +1137,7 @@
     <xf numFmtId="0" fontId="15" fillId="4" borderId="2" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="40% - 强调文字颜色 5 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
@@ -1887,7 +1961,7 @@
   <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E68" sqref="E68"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2043,7 +2117,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2273,8 +2347,8 @@
       <c r="C11" s="34">
         <v>10013</v>
       </c>
-      <c r="D11">
-        <v>-1</v>
+      <c r="D11" s="65" t="s">
+        <v>187</v>
       </c>
       <c r="E11">
         <v>10000</v>
@@ -2296,8 +2370,8 @@
       <c r="C12">
         <v>10012</v>
       </c>
-      <c r="D12">
-        <v>-1</v>
+      <c r="D12" s="65" t="s">
+        <v>188</v>
       </c>
       <c r="E12">
         <v>10000</v>
@@ -3346,7 +3420,7 @@
     <cfRule type="duplicateValues" dxfId="31" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3358,7 +3432,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="M2" sqref="M2"/>
+      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -5154,4 +5228,82 @@
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1EA8297-3C68-4CD9-BA33-D7773D7DFF85}">
+  <dimension ref="A4:E8"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="39.5" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="3" width="18.125" customWidth="1"/>
+    <col min="4" max="4" width="32.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A4" s="65" t="s">
+        <v>174</v>
+      </c>
+      <c r="B4" s="65" t="s">
+        <v>175</v>
+      </c>
+      <c r="C4" s="65" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A5" s="65" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A6" s="65" t="s">
+        <v>177</v>
+      </c>
+      <c r="C6" s="65" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A7" s="65" t="s">
+        <v>179</v>
+      </c>
+      <c r="B7" s="65" t="s">
+        <v>182</v>
+      </c>
+      <c r="C7" s="65" t="s">
+        <v>180</v>
+      </c>
+      <c r="D7" s="65" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A8" s="65" t="s">
+        <v>181</v>
+      </c>
+      <c r="B8" s="65" t="s">
+        <v>183</v>
+      </c>
+      <c r="C8" s="65" t="s">
+        <v>180</v>
+      </c>
+      <c r="D8" s="65" t="s">
+        <v>184</v>
+      </c>
+      <c r="E8" s="65" t="s">
+        <v>185</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="13" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
not force enumRef on interface
</commit_message>
<xml_diff>
--- a/example/config/ai_行为/ai行为.xlsx
+++ b/example/config/ai_行为/ai行为.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\work\mygit\cfggen\example\config\ai_行为\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D17AE943-A970-46DB-AD7D-607DEF58D9D9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9763FB4-B72E-4D48-B878-DC0C149913C3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5430" yWindow="3810" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5430" yWindow="3810" windowWidth="28800" windowHeight="15435" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="__CONFIG" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <sheet name="AI_ACTION_中文测试" sheetId="4" r:id="rId4"/>
     <sheet name="AI_ACTION_1_继续测试" sheetId="6" r:id="rId5"/>
     <sheet name="说明" sheetId="3" r:id="rId6"/>
-    <sheet name="TriggerTickType" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">AI_ACTION_中文测试!$C:$C</definedName>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="175">
   <si>
     <t>sheet</t>
   </si>
@@ -342,7 +341,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
-        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>出生后3</t>
@@ -352,7 +350,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
-        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>0秒</t>
@@ -475,7 +472,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
-        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>角色受伤(所有受伤状态，包括Buff</t>
@@ -485,7 +481,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
-        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>)</t>
@@ -497,7 +492,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
-        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>当前血量小于(百分比</t>
@@ -507,7 +501,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
-        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">) 例如20%  </t>
@@ -543,7 +536,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="宋体"/>
-        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>某一id召唤物全部消失时（包括被击杀、存活时间结束、玩家再次召唤时替换掉原有召唤物）</t>
@@ -553,7 +545,6 @@
         <sz val="11"/>
         <color rgb="FFFF0000"/>
         <rFont val="宋体"/>
-        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>只和与召唤者有关的行为配合使用，暂时只有行为3（暂时没有）</t>
@@ -613,7 +604,6 @@
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="宋体"/>
-        <charset val="134"/>
       </rPr>
       <t>为召唤者增加buff，</t>
     </r>
@@ -622,7 +612,6 @@
         <sz val="11"/>
         <color rgb="FFFF0000"/>
         <rFont val="宋体"/>
-        <charset val="134"/>
       </rPr>
       <t>只和条件3配合使用(暂时没有)</t>
     </r>
@@ -653,62 +642,6 @@
     <t>描述
 这里测试下多行效果
 再来一行</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>enumName</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>枚举名称</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>策划注释</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>参数列表</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>ConstValue</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>value:int</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>ByLevel</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>init:int</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>ByServerUpDay</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>角色等级相关</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>服务器启动天数</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>coefficient1:float</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>coefficient2:falot</t>
-    <phoneticPr fontId="13" type="noConversion"/>
-  </si>
-  <si>
-    <t>coefficient:float</t>
     <phoneticPr fontId="13" type="noConversion"/>
   </si>
   <si>
@@ -739,33 +672,28 @@
       <sz val="11"/>
       <color rgb="FFC00000"/>
       <name val="宋体"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="宋体"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="2"/>
       <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -773,49 +701,42 @@
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
       <color theme="1"/>
       <name val="微软雅黑"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="宋体"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <color indexed="9"/>
       <name val="宋体"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2115,7 +2036,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
     </sheetView>
@@ -2348,7 +2269,7 @@
         <v>10013</v>
       </c>
       <c r="D11" s="65" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
       <c r="E11">
         <v>10000</v>
@@ -2371,7 +2292,7 @@
         <v>10012</v>
       </c>
       <c r="D12" s="65" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="E12">
         <v>10000</v>
@@ -4966,7 +4887,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -5228,82 +5149,4 @@
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1EA8297-3C68-4CD9-BA33-D7773D7DFF85}">
-  <dimension ref="A4:E8"/>
-  <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="39.5" customWidth="1"/>
-    <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="18.125" customWidth="1"/>
-    <col min="4" max="4" width="32.625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A4" s="65" t="s">
-        <v>174</v>
-      </c>
-      <c r="B4" s="65" t="s">
-        <v>175</v>
-      </c>
-      <c r="C4" s="65" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A5" s="65" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A6" s="65" t="s">
-        <v>177</v>
-      </c>
-      <c r="C6" s="65" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A7" s="65" t="s">
-        <v>179</v>
-      </c>
-      <c r="B7" s="65" t="s">
-        <v>182</v>
-      </c>
-      <c r="C7" s="65" t="s">
-        <v>180</v>
-      </c>
-      <c r="D7" s="65" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A8" s="65" t="s">
-        <v>181</v>
-      </c>
-      <c r="B8" s="65" t="s">
-        <v>183</v>
-      </c>
-      <c r="C8" s="65" t="s">
-        <v>180</v>
-      </c>
-      <c r="D8" s="65" t="s">
-        <v>184</v>
-      </c>
-      <c r="E8" s="65" t="s">
-        <v>185</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="13" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>